<commit_message>
corrected 2 ed numbers and added one line
</commit_message>
<xml_diff>
--- a/etc/ap242/patches.xlsx
+++ b/etc/ap242/patches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="40" windowWidth="26180" windowHeight="16860" tabRatio="500"/>
+    <workbookView xWindow="840" yWindow="60" windowWidth="27880" windowHeight="16860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -613,8 +613,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="253">
+  <cellStyleXfs count="263">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -909,7 +919,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="253">
+  <cellStyles count="263">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -1036,6 +1046,11 @@
     <cellStyle name="Lien hypertexte" xfId="247" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="249" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="261" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -1162,6 +1177,11 @@
     <cellStyle name="Lien hypertexte visité" xfId="248" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="250" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="262" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
@@ -1783,7 +1803,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
final updates for CR11
</commit_message>
<xml_diff>
--- a/etc/ap242/patches.xlsx
+++ b/etc/ap242/patches.xlsx
@@ -51,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -100,62 +100,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Kevin Le Tutour:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This number is the last committed schema version on which the patch has been applied. 
-When equal to "x", it means the patch doesn't need to be applied to this specific schema (442 and/or 409 and/or 410 and/or ARM and/or MIM).</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Kevin Le Tutour:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This number is the last committed schema version on which the patch has been applied. 
-When equal to "x", it means the patch doesn't need to be applied to this specific schema (442 and/or 409 and/or 410 and/or ARM and/or MIM).</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="50">
   <si>
     <t>bug #</t>
   </si>
@@ -257,13 +207,6 @@
   </si>
   <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>&gt; replace mb3dgdt_additional_application_domain_enumeration by additional_application_domain_enumeration
-&gt; replace pmiwn3m_product_shape_type_enumeration by product_shape_type_enumeration
-&gt; replace pamap_initial_application_domain_enumeration by initial_application_domain_enumeration
-&gt; replace pamap_additional_application_domain_enumeration by additional_application_domain_enumeration
-&gt; replace pvd_life_cycle_stage_enumeration by life_cycle_stage_enumeration</t>
   </si>
   <si>
     <t>seems corrected</t>
@@ -352,7 +295,61 @@
 NB: concerns only characterized_resource_select used by Ressource_property</t>
   </si>
   <si>
-    <t>add:
+    <t>NO APPEAR : defined_data_name = SELECT</t>
+  </si>
+  <si>
+    <t>TYPE requirement_basis_select does appear in 410 lf - not needed for this one</t>
+  </si>
+  <si>
+    <t>Bug 5675 - Unknown type: MACHINING_FEATURE_DEFINITION</t>
+  </si>
+  <si>
+    <t>not a shtolo issue but too late to make a new version of AIC515 in CR11</t>
+  </si>
+  <si>
+    <t>Replace:
+FUNCTION is_coordinate_property(
+...
+end_function
+by:
+FUNCTION is_coordinate_property(
+               arg : specified_general_property
+           ) : BOOLEAN;
+(* this line 
+    IF
+'AP209_MULTIDISCIPLINARY_ANALYSIS_AND_DESIGN_MIM_LF.EXTERNALLY_DEFINED_ITEM' IN
+TYPEOF( arg ) THEN
+   is replaced by the following two lines as patch for BZ#5019 *)
+    IF ('AP209_MULTIDISCIPLINARY_ANALYSIS_AND_DESIGN_MIM_LF.EXTERNALLY_DEFINED_ITEM' IN TYPEOF(arg\specified_general_property.name_specifier) ) THEN  
+      RETURN( TRUE );
+    END_IF;
+(* this line 
+    RETURN(
+'AP209_MULTIDISCIPLINARY_ANALYSIS_AND_DESIGN_MIM_LF.COORDINATE_DATA_NAME' IN
+TYPEOF( arg ) );
+   is replaced by the following section as patch for BZ#5019 and BZ#5054
+    RETURN
+('AP209_MULTIDISCIPLINARY_ANALYSIS_AND_DESIGN_MIM_LF.COORDINATE_DATA_NAME' IN
+    TYPEOF(arg\specified_general_property.name_specifier)); *)
+    IF (arg\specified_general_property.name_specifier = PROPERTY_3D_DATA_NAME.POSITION) OR ('AP209_MULTIDISCIPLINARY_ANALYSIS_AND_DESIGN_MIM_LF.COORDINATE_DATA_NAME' IN TYPEOF(arg\specified_general_property.name_specifier)) THEN 
+       RETURN ( TRUE );
+    ELSE
+       RETURN( FALSE );
+    END_IF;
+END_FUNCTION;</t>
+  </si>
+  <si>
+    <t>Replace:
+TYPE csg_primitive = SELECT (
+   block,
+   bounded_primitive_2d,
+   right_angular_wedge,
+   right_circular_cone,
+   right_circular_cylinder,
+   sphere,
+   torus);
+END_TYPE;
+by:
 TYPE csg_primitive = SELECT (
    block,
    bounded_primitive_2d,
@@ -491,57 +488,20 @@
    END_REPEAT;
    RETURN(TRUE);
 END_FUNCTION; 
-(* End of added FUNCTIONs.klt 2015-09-28 *)</t>
-  </si>
-  <si>
-    <t>NO APPEAR : defined_data_name = SELECT</t>
-  </si>
-  <si>
-    <t>TYPE requirement_basis_select does appear in 410 lf - not needed for this one</t>
-  </si>
-  <si>
-    <t>Done in P409 mim_lf.exp as proposed with this result:
-  FUNCTION is_coordinate_property(
-               arg : specified_general_property
-           ) : BOOLEAN;
-(* this line 
-    IF
-'AP209_MULTIDISCIPLINARY_ANALYSIS_AND_DESIGN_MIM_LF.EXTERNALLY_DEFINED_ITEM' IN
-TYPEOF( arg ) THEN
-   is replaced by the following two lines as patch for BZ#5019 *)
-    IF
-('AP209_MULTIDISCIPLINARY_ANALYSIS_AND_DESIGN_MIM_LF.EXTERNALLY_DEFINED_ITEM'
-IN
-        TYPEOF(arg\specified_general_property.name_specifier) ) THEN  
-      RETURN( TRUE );
-    END_IF;
-(* this line 
-    RETURN(
-'AP209_MULTIDISCIPLINARY_ANALYSIS_AND_DESIGN_MIM_LF.COORDINATE_DATA_NAME' IN
-TYPEOF( arg ) );
-   is replaced by the following section as patch for BZ#5019 and BZ#5054
-    RETURN
-('AP209_MULTIDISCIPLINARY_ANALYSIS_AND_DESIGN_MIM_LF.COORDINATE_DATA_NAME' IN
-    TYPEOF(arg\specified_general_property.name_specifier)); *)
-    IF (arg\specified_general_property.name_specifier =
-PROPERTY_3D_DATA_NAME.POSITION)
-        OR
-('AP209_MULTIDISCIPLINARY_ANALYSIS_AND_DESIGN_MIM_LF.COORDINATE_DATA_NAME' IN
-        TYPEOF(arg\specified_general_property.name_specifier)) THEN 
-       RETURN ( TRUE );
-    ELSE
-       RETURN( FALSE );
-    END_IF;
-  END_FUNCTION;</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Bug 5675 - Unknown type: MACHINING_FEATURE_DEFINITION</t>
-  </si>
-  <si>
-    <t>not a shtolo issue but too late to make a new version of AIC515 in CR11</t>
+(* End of added FUNCTIONs. klt 2015-09-30 *)</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>FOR THE 3 LFs:
+&gt; replace mb3dgdt_additional_application_domain_enumeration by additional_application_domain_enumeration
+&gt; replace pmiwn3m_product_shape_type_enumeration by product_shape_type_enumeration
+&gt; replace pamap_initial_application_domain_enumeration by initial_application_domain_enumeration
+&gt; replace pamap_additional_application_domain_enumeration by additional_application_domain_enumeration
+&gt; replace pvd_life_cycle_stage_enumeration by life_cycle_stage_enumeration
+ONLY FOR 410:
+&gt; replace ps_initial_application_domain_enumeration by initial_application_domain_enumeration</t>
   </si>
 </sst>
 </file>
@@ -616,8 +576,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="269">
+  <cellStyleXfs count="301">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -928,7 +920,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="269">
+  <cellStyles count="301">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -1063,6 +1055,22 @@
     <cellStyle name="Lien hypertexte" xfId="263" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="265" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="299" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -1197,6 +1205,22 @@
     <cellStyle name="Lien hypertexte visité" xfId="264" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="266" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="300" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
@@ -1818,7 +1842,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1837,7 +1861,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="16" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1867,13 +1891,13 @@
         <v>7</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="16" customHeight="1">
@@ -1889,20 +1913,20 @@
       <c r="D2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="6">
-        <v>1.38</v>
+      <c r="E2" s="14">
+        <v>1.4</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>23</v>
       </c>
       <c r="G2" s="6">
-        <v>1.64</v>
+        <v>1.67</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>23</v>
       </c>
       <c r="I2" s="6">
-        <v>1.31</v>
+        <v>1.33</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>23</v>
@@ -1911,7 +1935,7 @@
         <v>8</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M2" s="4"/>
     </row>
@@ -1928,29 +1952,29 @@
       <c r="D3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="6">
-        <v>1.38</v>
+      <c r="E3" s="14">
+        <v>1.4</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>23</v>
       </c>
       <c r="G3" s="6">
-        <v>1.64</v>
+        <v>1.67</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>23</v>
       </c>
       <c r="I3" s="6">
-        <v>1.31</v>
+        <v>1.33</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>23</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M3" s="4"/>
     </row>
@@ -1967,8 +1991,8 @@
       <c r="D4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="6">
-        <v>1.38</v>
+      <c r="E4" s="14">
+        <v>1.4</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>23</v>
@@ -1980,7 +2004,7 @@
         <v>23</v>
       </c>
       <c r="I4" s="6">
-        <v>1.31</v>
+        <v>1.33</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>23</v>
@@ -1989,10 +2013,10 @@
         <v>13</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="16" customHeight="1">
@@ -2012,25 +2036,25 @@
         <v>23</v>
       </c>
       <c r="F5" s="6">
-        <v>1.45</v>
+        <v>1.47</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="H5" s="6">
-        <v>1.66</v>
+        <v>1.68</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J5" s="14">
-        <v>1.5</v>
+        <v>1.52</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>14</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M5" s="4"/>
     </row>
@@ -2051,19 +2075,19 @@
         <v>23</v>
       </c>
       <c r="F6" s="6">
-        <v>1.45</v>
+        <v>1.47</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>23</v>
       </c>
       <c r="H6" s="6">
-        <v>1.66</v>
+        <v>1.68</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J6" s="14">
-        <v>1.5</v>
+        <v>1.52</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>16</v>
@@ -2079,7 +2103,7 @@
         <v>4619</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>20</v>
@@ -2189,10 +2213,18 @@
       <c r="F10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="K10" s="11"/>
       <c r="L10" s="6"/>
       <c r="M10" s="4"/>
@@ -2205,7 +2237,7 @@
         <v>4904</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>19</v>
@@ -2223,16 +2255,16 @@
         <v>23</v>
       </c>
       <c r="I11" s="6">
-        <v>1.31</v>
+        <v>1.33</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>23</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M11" s="4"/>
     </row>
@@ -2250,9 +2282,15 @@
       <c r="E12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="I12" s="6" t="s">
         <v>23</v>
       </c>
@@ -2272,7 +2310,7 @@
         <v>4988</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>20</v>
@@ -2297,7 +2335,7 @@
       </c>
       <c r="L13" s="6"/>
       <c r="M13" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="16" customHeight="1">
@@ -2327,7 +2365,7 @@
       <c r="J14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="16" customHeight="1">
@@ -2392,7 +2430,7 @@
       </c>
       <c r="L16" s="6"/>
       <c r="M16" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="16" customHeight="1">
@@ -2459,7 +2497,7 @@
       </c>
       <c r="L18" s="6"/>
       <c r="M18" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="16" customHeight="1">
@@ -2493,7 +2531,7 @@
       </c>
       <c r="L19" s="6"/>
       <c r="M19" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="16" customHeight="1">
@@ -2523,13 +2561,13 @@
         <v>23</v>
       </c>
       <c r="J20" s="14">
-        <v>1.5</v>
+        <v>1.52</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M20" s="4"/>
     </row>
@@ -2560,16 +2598,16 @@
         <v>23</v>
       </c>
       <c r="J21" s="14">
-        <v>1.5</v>
+        <v>1.52</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="16" customHeight="1">
@@ -2635,7 +2673,7 @@
         <v>23</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L23" s="6"/>
       <c r="M23" s="4"/>
@@ -2667,16 +2705,16 @@
         <v>23</v>
       </c>
       <c r="J24" s="14">
-        <v>1.5</v>
+        <v>1.52</v>
       </c>
       <c r="K24" s="10" t="s">
         <v>46</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="16" customHeight="1">
@@ -2694,7 +2732,7 @@
         <v>23</v>
       </c>
       <c r="F25" s="6">
-        <v>1.45</v>
+        <v>1.47</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>23</v>
@@ -2706,16 +2744,16 @@
         <v>23</v>
       </c>
       <c r="J25" s="14">
-        <v>1.5</v>
+        <v>1.52</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="16" customHeight="1">
@@ -2792,7 +2830,7 @@
         <v>5587</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>20</v>
@@ -2827,7 +2865,7 @@
         <v>5588</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>20</v>
@@ -2862,7 +2900,7 @@
         <v>5675</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>21</v>
@@ -2888,7 +2926,7 @@
       <c r="K30" s="11"/>
       <c r="L30" s="6"/>
       <c r="M30" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="16" customHeight="1">

</xml_diff>

<commit_message>
updated for bug 5004
</commit_message>
<xml_diff>
--- a/etc/ap242/patches.xlsx
+++ b/etc/ap242/patches.xlsx
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="58">
   <si>
     <t>bug #</t>
   </si>
@@ -261,15 +261,6 @@
       velocity,
       vorticity );
   END_TYPE;  </t>
-  </si>
-  <si>
-    <t>Fixed as patch to 449ed2:
-  TYPE tuple_space = SELECT
-    ( product_space,
-(* next line added as patch for BZ#5023 *)
-      mesh_derived_maths_space,
-     extended_tuple_space );
-  END_TYPE;</t>
   </si>
   <si>
     <t>patch id</t>
@@ -503,12 +494,70 @@
 ONLY FOR 410:
 &gt; replace ps_initial_application_domain_enumeration by initial_application_domain_enumeration</t>
   </si>
+  <si>
+    <t>replace tuple space type by:
+  TYPE tuple_space = SELECT
+    ( product_space,
+(* next line added as patch for BZ#5023 *)
+      mesh_derived_maths_space,
+     extended_tuple_space );
+  END_TYPE;</t>
+  </si>
+  <si>
+    <t>Bug 4979 - patch 409 longform for explicit_unstructured_mesh.cells syntax error</t>
+  </si>
+  <si>
+    <t>Bug 4847 - manual editing of html needed</t>
+  </si>
+  <si>
+    <t>Bug 4992 - Patch 409, 410 mim longforms to add 209, 210 specific ap rule</t>
+  </si>
+  <si>
+    <t>Bug 4994 - patch 409 ARM longform to correct product_of_mesh.wr1</t>
+  </si>
+  <si>
+    <t>Bug 4978 - patch for associated_definition bug</t>
+  </si>
+  <si>
+    <t>Bug 5004 - patch 409, 410, 442 MIM longform missing MACHINING_FEATURE_DEFINITION TYPE</t>
+  </si>
+  <si>
+    <t>Bug 5672 - Running STEP Tools Express Checker on AP242ed2 AIM long form schema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add this type from ed1 of 442 : 
+(* BZ#5004 *)
+TYPE machining_feature_definition = SELECT (
+  boss,
+  compound_feature,
+  externally_defined_feature_definition,
+  flat_face,
+  gear,
+  marking,
+  outer_round,
+  outside_profile,
+  pocket,
+  protrusion,
+  removal_volume,
+  replicate_feature,
+  revolved_profile,
+  rib_top,
+  round_hole,
+  rounded_end,
+  spherical_cap,
+  step,
+  slot,
+  thread,
+  turned_knurl);
+END_TYPE;
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -558,13 +607,24 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -576,7 +636,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="301">
+  <cellStyleXfs count="317">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -878,8 +938,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -919,8 +995,17 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="301">
+  <cellStyles count="317">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -1071,6 +1156,14 @@
     <cellStyle name="Lien hypertexte" xfId="295" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="297" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="315" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -1221,6 +1314,14 @@
     <cellStyle name="Lien hypertexte visité" xfId="296" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="298" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="316" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
@@ -1841,8 +1942,8 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1861,7 +1962,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="16" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1891,13 +1992,13 @@
         <v>7</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="16" customHeight="1">
@@ -1935,7 +2036,7 @@
         <v>8</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M2" s="4"/>
     </row>
@@ -1971,10 +2072,10 @@
         <v>23</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M3" s="4"/>
     </row>
@@ -2013,10 +2114,10 @@
         <v>13</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="16" customHeight="1">
@@ -2054,7 +2155,7 @@
         <v>14</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M5" s="4"/>
     </row>
@@ -2261,10 +2362,10 @@
         <v>23</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M11" s="4"/>
     </row>
@@ -2564,10 +2665,10 @@
         <v>1.52</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M20" s="4"/>
     </row>
@@ -2604,10 +2705,10 @@
         <v>34</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="16" customHeight="1">
@@ -2708,13 +2809,13 @@
         <v>1.52</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="16" customHeight="1">
@@ -2747,13 +2848,13 @@
         <v>1.52</v>
       </c>
       <c r="K25" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="L25" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="L25" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="M25" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="16" customHeight="1">
@@ -2900,7 +3001,7 @@
         <v>5675</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>21</v>
@@ -2926,21 +3027,40 @@
       <c r="K30" s="11"/>
       <c r="L30" s="6"/>
       <c r="M30" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="16" customHeight="1">
       <c r="A31" s="6">
         <v>30</v>
       </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
+      <c r="B31" s="6">
+        <v>4979</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="K31" s="11"/>
       <c r="L31" s="6"/>
       <c r="M31" s="4"/>
@@ -2949,14 +3069,33 @@
       <c r="A32" s="6">
         <v>31</v>
       </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
+      <c r="B32" s="6">
+        <v>4847</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="L32" s="6"/>
       <c r="M32" s="4"/>
     </row>
@@ -2964,14 +3103,33 @@
       <c r="A33" s="6">
         <v>32</v>
       </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
+      <c r="B33" s="6">
+        <v>4992</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="L33" s="6"/>
       <c r="M33" s="4"/>
     </row>
@@ -2979,14 +3137,33 @@
       <c r="A34" s="6">
         <v>33</v>
       </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
+      <c r="B34" s="6">
+        <v>4994</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="L34" s="6"/>
       <c r="M34" s="4"/>
     </row>
@@ -2994,14 +3171,33 @@
       <c r="A35" s="6">
         <v>34</v>
       </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
+      <c r="B35" s="6">
+        <v>4978</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="L35" s="6"/>
       <c r="M35" s="4"/>
     </row>
@@ -3009,14 +3205,36 @@
       <c r="A36" s="6">
         <v>35</v>
       </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
+      <c r="B36" s="6">
+        <v>5004</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F36" s="17">
+        <v>1.48</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H36" s="17">
+        <v>1.69</v>
+      </c>
+      <c r="I36" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J36" s="6">
+        <v>1.53</v>
+      </c>
+      <c r="K36" s="16" t="s">
+        <v>57</v>
+      </c>
       <c r="L36" s="6"/>
       <c r="M36" s="4"/>
     </row>
@@ -3024,14 +3242,33 @@
       <c r="A37" s="6">
         <v>36</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
+      <c r="B37" s="6">
+        <v>5672</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="L37" s="6"/>
       <c r="M37" s="4"/>
     </row>

</xml_diff>

<commit_message>
added Patch Bug 5493
</commit_message>
<xml_diff>
--- a/etc/ap242/patches.xlsx
+++ b/etc/ap242/patches.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klt/Projets/EclipseWS2/stepmod/etc/ap242/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Issue list" sheetId="1" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="88">
   <si>
     <t>bug #</t>
   </si>
@@ -593,6 +598,17 @@
   <si>
     <t>Bug 5706</t>
   </si>
+  <si>
+    <t>Bug 5493 - Extend data_environment for dimensional_characteristic_representation and others</t>
+  </si>
+  <si>
+    <t>change data_environment.elements as :
+ENTITY data_environment;
+  name : label;
+  description : text;
+  elements : SET [1:?] OF property_definition_representation;
+END_ENTITY;</t>
+  </si>
 </sst>
 </file>
 
@@ -1176,456 +1192,456 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="451">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="137" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="139" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="141" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="143" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="145" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="147" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="149" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="151" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="153" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="155" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="157" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="159" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="161" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="163" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="165" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="167" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="169" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="171" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="173" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="175" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="177" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="179" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="181" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="183" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="185" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="187" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="189" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="191" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="193" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="195" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="197" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="199" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="201" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="203" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="205" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="207" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="209" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="211" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="213" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="215" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="217" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="219" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="221" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="223" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="225" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="227" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="229" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="231" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="233" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="235" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="237" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="239" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="241" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="243" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="245" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="247" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="249" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="251" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="253" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="255" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="257" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="259" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="261" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="263" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="265" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="267" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="269" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="271" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="273" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="275" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="277" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="279" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="281" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="283" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="285" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="287" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="289" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="291" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="293" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="295" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="297" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="299" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="301" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="303" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="305" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="307" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="309" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="311" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="313" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="315" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="317" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="319" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="321" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="323" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="325" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="327" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="329" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="331" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="333" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="335" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="337" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="339" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="341" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="343" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="345" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="347" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="349" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="351" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="353" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="355" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="357" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="359" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="361" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="363" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="365" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="367" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="369" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="371" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="373" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="375" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="377" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="379" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="381" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="383" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="385" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="387" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="389" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="391" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="393" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="395" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="397" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="399" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="401" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="403" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="405" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="407" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="409" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="411" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="413" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="415" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="417" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="419" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="421" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="423" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="425" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="427" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="429" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="431" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="433" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="435" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="437" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="439" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="441" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="443" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="445" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="447" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="449" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="158" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="160" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="162" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="164" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="166" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="168" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="170" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="172" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="174" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="176" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="178" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="180" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="182" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="184" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="186" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="188" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="190" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="192" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="194" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="196" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="198" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="200" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="202" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="204" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="206" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="208" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="210" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="212" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="214" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="216" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="218" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="220" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="222" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="224" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="226" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="228" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="230" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="232" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="234" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="236" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="238" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="240" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="242" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="244" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="246" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="248" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="250" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="252" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="254" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="256" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="258" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="260" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="262" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="264" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="266" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="268" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="270" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="272" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="274" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="276" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="278" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="280" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="282" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="284" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="286" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="288" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="290" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="292" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="294" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="296" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="298" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="300" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="302" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="304" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="306" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="308" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="310" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="312" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="314" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="316" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="318" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="320" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="322" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="324" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="326" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="328" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="330" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="332" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="334" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="336" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="338" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="340" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="342" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="344" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="346" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="348" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="350" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="352" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="354" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="356" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="358" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="360" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="362" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="364" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="366" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="368" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="370" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="372" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="374" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="376" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="378" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="380" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="382" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="384" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="386" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="388" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="390" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="392" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="394" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="396" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="398" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="400" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="402" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="404" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="406" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="408" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="410" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="412" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="414" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="416" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="418" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="420" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="422" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="424" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="426" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="428" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="430" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="432" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="434" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="436" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="438" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="440" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="442" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="444" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="446" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="448" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
@@ -1897,12 +1913,17 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:M39" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:M39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:M40" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A1:M40"/>
   <tableColumns count="13">
     <tableColumn id="1" name="patch id" dataDxfId="12"/>
     <tableColumn id="2" name="bug #" dataDxfId="11"/>
@@ -2244,19 +2265,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.83203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="11" style="7" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="7" customWidth="1"/>
     <col min="5" max="5" width="13.5" style="5" customWidth="1"/>
     <col min="6" max="10" width="13.5" style="4" customWidth="1"/>
     <col min="11" max="11" width="69.33203125" style="11" customWidth="1"/>
@@ -2265,7 +2286,7 @@
     <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="16" customHeight="1">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
@@ -2306,7 +2327,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16" customHeight="1">
+    <row r="2" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -2345,7 +2366,7 @@
       </c>
       <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:13" ht="16" customHeight="1">
+    <row r="3" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -2384,7 +2405,7 @@
       </c>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:13" ht="16" customHeight="1">
+    <row r="4" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -2425,7 +2446,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="16" customHeight="1">
+    <row r="5" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -2464,7 +2485,7 @@
       </c>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="1:13" ht="16" customHeight="1">
+    <row r="6" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -2501,7 +2522,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:13" ht="16" customHeight="1">
+    <row r="7" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -2535,7 +2556,7 @@
       <c r="L7" s="6"/>
       <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="1:13" ht="16" customHeight="1">
+    <row r="8" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -2569,7 +2590,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:13" ht="16" customHeight="1">
+    <row r="9" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -2603,7 +2624,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="1:13" ht="16" customHeight="1">
+    <row r="10" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -2637,7 +2658,7 @@
       <c r="L10" s="6"/>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:13" ht="17" customHeight="1">
+    <row r="11" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -2676,7 +2697,7 @@
       </c>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:13" ht="16" customHeight="1">
+    <row r="12" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -2712,7 +2733,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="16" customHeight="1">
+    <row r="13" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -2748,7 +2769,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="16" customHeight="1">
+    <row r="14" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -2787,7 +2808,7 @@
       </c>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="1:13" ht="16" customHeight="1">
+    <row r="15" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -2821,7 +2842,7 @@
       <c r="L15" s="6"/>
       <c r="M15" s="4"/>
     </row>
-    <row r="16" spans="1:13" ht="16" customHeight="1">
+    <row r="16" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -2857,7 +2878,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="16" customHeight="1">
+    <row r="17" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -2891,7 +2912,7 @@
       <c r="L17" s="6"/>
       <c r="M17" s="4"/>
     </row>
-    <row r="18" spans="1:13" ht="16" customHeight="1">
+    <row r="18" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -2927,7 +2948,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="16" customHeight="1">
+    <row r="19" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -2963,7 +2984,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="16" customHeight="1">
+    <row r="20" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -3002,7 +3023,7 @@
       </c>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="1:13" ht="16" customHeight="1">
+    <row r="21" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -3043,7 +3064,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="16" customHeight="1">
+    <row r="22" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -3077,7 +3098,7 @@
       <c r="L22" s="6"/>
       <c r="M22" s="4"/>
     </row>
-    <row r="23" spans="1:13" ht="16" customHeight="1">
+    <row r="23" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -3114,7 +3135,7 @@
       <c r="L23" s="6"/>
       <c r="M23" s="4"/>
     </row>
-    <row r="24" spans="1:13" ht="16" customHeight="1">
+    <row r="24" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -3155,7 +3176,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="16" customHeight="1">
+    <row r="25" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -3196,7 +3217,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="16" customHeight="1">
+    <row r="26" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -3230,7 +3251,7 @@
       <c r="L26" s="6"/>
       <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="1:13" ht="16" customHeight="1">
+    <row r="27" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -3264,7 +3285,7 @@
       <c r="L27" s="6"/>
       <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="1:13" ht="16" customHeight="1">
+    <row r="28" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -3298,7 +3319,7 @@
       <c r="L28" s="6"/>
       <c r="M28" s="4"/>
     </row>
-    <row r="29" spans="1:13" ht="16" customHeight="1">
+    <row r="29" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -3332,7 +3353,7 @@
       <c r="L29" s="6"/>
       <c r="M29" s="4"/>
     </row>
-    <row r="30" spans="1:13" ht="16" customHeight="1">
+    <row r="30" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -3368,7 +3389,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="16" customHeight="1">
+    <row r="31" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -3402,7 +3423,7 @@
       <c r="L31" s="6"/>
       <c r="M31" s="4"/>
     </row>
-    <row r="32" spans="1:13" ht="16" customHeight="1">
+    <row r="32" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -3436,7 +3457,7 @@
       <c r="L32" s="6"/>
       <c r="M32" s="4"/>
     </row>
-    <row r="33" spans="1:13" ht="16" customHeight="1">
+    <row r="33" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -3470,7 +3491,7 @@
       <c r="L33" s="6"/>
       <c r="M33" s="4"/>
     </row>
-    <row r="34" spans="1:13" ht="16" customHeight="1">
+    <row r="34" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>33</v>
       </c>
@@ -3504,7 +3525,7 @@
       <c r="L34" s="6"/>
       <c r="M34" s="4"/>
     </row>
-    <row r="35" spans="1:13" ht="16" customHeight="1">
+    <row r="35" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>34</v>
       </c>
@@ -3538,7 +3559,7 @@
       <c r="L35" s="6"/>
       <c r="M35" s="4"/>
     </row>
-    <row r="36" spans="1:13" ht="16" customHeight="1">
+    <row r="36" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>35</v>
       </c>
@@ -3577,7 +3598,7 @@
       </c>
       <c r="M36" s="4"/>
     </row>
-    <row r="37" spans="1:13" ht="16" customHeight="1">
+    <row r="37" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -3611,7 +3632,7 @@
       <c r="L37" s="6"/>
       <c r="M37" s="4"/>
     </row>
-    <row r="38" spans="1:13" ht="16" customHeight="1">
+    <row r="38" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>37</v>
       </c>
@@ -3650,7 +3671,7 @@
       </c>
       <c r="M38" s="4"/>
     </row>
-    <row r="39" spans="1:13" ht="16" customHeight="1">
+    <row r="39" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>38</v>
       </c>
@@ -3683,6 +3704,43 @@
       </c>
       <c r="L39" s="6"/>
       <c r="M39" s="4"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="6">
+        <v>39</v>
+      </c>
+      <c r="B40" s="6">
+        <v>5493</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F40" s="6">
+        <v>1.49</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="6">
+        <v>1.71</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J40" s="6">
+        <v>1.58</v>
+      </c>
+      <c r="K40" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="L40" s="6"/>
+      <c r="M40" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3690,11 +3748,6 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3706,24 +3759,24 @@
       <selection activeCell="D6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" style="1" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" s="18" t="s">
         <v>74</v>
       </c>
@@ -3731,7 +3784,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" s="18" t="s">
         <v>18</v>
       </c>
@@ -3739,7 +3792,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" s="18" t="s">
         <v>19</v>
       </c>
@@ -3747,7 +3800,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" s="18" t="s">
         <v>73</v>
       </c>
@@ -3755,7 +3808,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
@@ -3775,17 +3828,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>81</v>
       </c>
@@ -3793,10 +3846,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>